<commit_message>
Continued on home page. Put a screenshot. Put some data at the back
</commit_message>
<xml_diff>
--- a/protected/data/Initializers/GoalBookData.xlsx
+++ b/protected/data/Initializers/GoalBookData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tremmillicious\Documents\Projects\GoalBook\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\goalbook\protected\data\Initializers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="7" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="Todo" sheetId="9" r:id="rId10"/>
     <sheet name="GoalAssignment" sheetId="3" r:id="rId11"/>
     <sheet name="GoalList" sheetId="11" r:id="rId12"/>
-    <sheet name="Sheet4" sheetId="13" r:id="rId13"/>
+    <sheet name="GoalCommitment" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="900">
   <si>
     <t>Active</t>
   </si>
@@ -2716,6 +2716,21 @@
   </si>
   <si>
     <t>0001-01-01 00:00:17</t>
+  </si>
+  <si>
+    <t>owner_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least invite a lady for a 3 course meal for dinner </t>
+  </si>
+  <si>
+    <t>Cooking a big meal</t>
+  </si>
+  <si>
+    <t>2014-01-02 00:00:16</t>
+  </si>
+  <si>
+    <t>0001-01-01 00:00:18</t>
   </si>
 </sst>
 </file>
@@ -4485,12 +4500,48 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B1" t="s">
+        <v>895</v>
+      </c>
+      <c r="C1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4693,8 +4744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E711"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A238" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16924,7 +16975,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17228,10 +17279,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17425,8 +17476,8 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>584</v>
+      <c r="B7" s="1">
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -17657,8 +17708,8 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>584</v>
+      <c r="B15" s="1">
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>715</v>
@@ -17911,6 +17962,35 @@
         <v>894</v>
       </c>
       <c r="I23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="E24" s="2">
+        <v>15</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>898</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>899</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>899</v>
+      </c>
+      <c r="I24" s="2">
         <v>1</v>
       </c>
     </row>
@@ -17927,7 +18007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working on the goal page. Now selecting the goals in bank
</commit_message>
<xml_diff>
--- a/protected/data/Initializers/GoalBookData.xlsx
+++ b/protected/data/Initializers/GoalBookData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="907">
   <si>
     <t>Active</t>
   </si>
@@ -2731,6 +2731,27 @@
   </si>
   <si>
     <t>0001-01-01 00:00:18</t>
+  </si>
+  <si>
+    <t>Lose Weight</t>
+  </si>
+  <si>
+    <t>Eat Healthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking Acomplishments </t>
+  </si>
+  <si>
+    <t>Update your Skills</t>
+  </si>
+  <si>
+    <t>Speak English fluently</t>
+  </si>
+  <si>
+    <t>1000 subscribers to my blogs</t>
+  </si>
+  <si>
+    <t>Donate at an organisation</t>
   </si>
 </sst>
 </file>
@@ -4742,10 +4763,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E711"/>
+  <dimension ref="A1:E720"/>
   <sheetViews>
-    <sheetView topLeftCell="A238" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C252" sqref="C252"/>
+    <sheetView tabSelected="1" topLeftCell="A702" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D725" sqref="D725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16840,6 +16861,159 @@
         <v>584</v>
       </c>
       <c r="E711" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="712" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A712" s="3">
+        <v>711</v>
+      </c>
+      <c r="B712" s="1">
+        <v>6</v>
+      </c>
+      <c r="C712" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="D712" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E712" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A713" s="3">
+        <v>712</v>
+      </c>
+      <c r="B713" s="1">
+        <v>6</v>
+      </c>
+      <c r="C713" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D713" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E713" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="714" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A714" s="3">
+        <v>713</v>
+      </c>
+      <c r="B714" s="1">
+        <v>8</v>
+      </c>
+      <c r="C714" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D714" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E714" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A715" s="3">
+        <v>714</v>
+      </c>
+      <c r="B715" s="1">
+        <v>8</v>
+      </c>
+      <c r="C715" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D715" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E715" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A716" s="3">
+        <v>715</v>
+      </c>
+      <c r="B716" s="1">
+        <v>8</v>
+      </c>
+      <c r="C716" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="D716" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E716" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A717" s="3">
+        <v>716</v>
+      </c>
+      <c r="B717" s="1">
+        <v>8</v>
+      </c>
+      <c r="C717" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D717" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E717" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A718" s="3">
+        <v>717</v>
+      </c>
+      <c r="B718" s="1">
+        <v>10</v>
+      </c>
+      <c r="C718" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D718" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E718" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A719" s="3">
+        <v>718</v>
+      </c>
+      <c r="B719" s="1">
+        <v>7</v>
+      </c>
+      <c r="C719" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="D719" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E719" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A720" s="3">
+        <v>719</v>
+      </c>
+      <c r="B720" s="1">
+        <v>12</v>
+      </c>
+      <c r="C720" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D720" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E720" s="3" t="s">
         <v>584</v>
       </c>
     </row>
@@ -16975,7 +17149,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="A7:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17281,8 +17455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added some of the goal page staff like goal level. Made sure that each page, goal skill will diplay its goal type and category
</commit_message>
<xml_diff>
--- a/protected/data/Initializers/GoalBookData.xlsx
+++ b/protected/data/Initializers/GoalBookData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="7" r:id="rId1"/>
@@ -23,15 +23,16 @@
     <sheet name="TodoCategory" sheetId="8" r:id="rId9"/>
     <sheet name="Todo" sheetId="9" r:id="rId10"/>
     <sheet name="GoalAssignment" sheetId="3" r:id="rId11"/>
-    <sheet name="GoalList" sheetId="11" r:id="rId12"/>
-    <sheet name="GoalCommitment" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId12"/>
+    <sheet name="GoalList" sheetId="11" r:id="rId13"/>
+    <sheet name="GoalCommitment" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="912">
   <si>
     <t>Active</t>
   </si>
@@ -2752,6 +2753,21 @@
   </si>
   <si>
     <t>Donate at an organisation</t>
+  </si>
+  <si>
+    <t>Goals Achieved</t>
+  </si>
+  <si>
+    <t>Goals to Maintain</t>
+  </si>
+  <si>
+    <t>Goals to Apply</t>
+  </si>
+  <si>
+    <t>Dream Goals</t>
+  </si>
+  <si>
+    <t>Insipring Words</t>
   </si>
 </sst>
 </file>
@@ -4091,10 +4107,22 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4519,7 +4547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -4765,7 +4793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A702" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A714" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D725" sqref="D725"/>
     </sheetView>
   </sheetViews>
@@ -17028,10 +17056,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17138,6 +17166,90 @@
         <v>584</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>603</v>
+      </c>
+      <c r="C8" t="s">
+        <v>907</v>
+      </c>
+      <c r="D8" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>603</v>
+      </c>
+      <c r="C9" t="s">
+        <v>908</v>
+      </c>
+      <c r="D9" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" t="s">
+        <v>909</v>
+      </c>
+      <c r="D10" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>603</v>
+      </c>
+      <c r="C11" t="s">
+        <v>910</v>
+      </c>
+      <c r="D11" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>603</v>
+      </c>
+      <c r="C12" t="s">
+        <v>911</v>
+      </c>
+      <c r="D12" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>603</v>
+      </c>
+      <c r="C13" t="s">
+        <v>591</v>
+      </c>
+      <c r="D13" t="s">
+        <v>584</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17149,7 +17261,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A7:D14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Put a discussion and message modules. Eliminate some of the colors. Pettified UI
</commit_message>
<xml_diff>
--- a/protected/data/Initializers/GoalBookData.xlsx
+++ b/protected/data/Initializers/GoalBookData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7890" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="7" r:id="rId1"/>
@@ -17058,7 +17058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -17260,7 +17260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>